<commit_message>
fixes to the pop file
</commit_message>
<xml_diff>
--- a/data/epi_data_Australia.xlsx
+++ b/data/epi_data_Australia.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\covasim-australia\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/covasim-australia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{197884F1-230A-49B0-9BD2-75085DC5529A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFC586D-3230-D746-BED7-F324316F3088}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="epi_data_Australia" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -994,19 +994,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K129"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:K257"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>5049</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>4026</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>8589</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>5521</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>9205</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>8228</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>5316</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>10100</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>14430</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>16758</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>16640</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>16984</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>18437</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>13125</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>14804</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>16186</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>20018</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>14511</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>14249</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>7071</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>12830</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>9152</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>11401</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>14430</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>5723</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>21420</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>11632</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>5528</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>33426</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>9861</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>12392</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>8480</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>8126</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>5850</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>5818</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>5148</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>9683</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>6768</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>6768</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>9140</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>3752</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>4181</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>9955</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>6348</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>8793</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>9529</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>8339</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>5030</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>8931</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>12400</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>14671</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>9504</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>6314</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>8149</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>20999</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>20304</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>20168</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>22103</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>17954</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>15381</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>17416</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>20682</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>11</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>26320</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>24430</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>25553</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>21597</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -5703,6 +5703,390 @@
       <c r="K129">
         <v>24528</v>
       </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D130" s="1"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D131" s="1"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D132" s="1"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D133" s="1"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D134" s="1"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D135" s="1"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D136" s="1"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D137" s="1"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D138" s="1"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D139" s="1"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D140" s="1"/>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D141" s="1"/>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D142" s="1"/>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D143" s="1"/>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D144" s="1"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D145" s="1"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D146" s="1"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D147" s="1"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D148" s="1"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D149" s="1"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D150" s="1"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D151" s="1"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D152" s="1"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D153" s="1"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D154" s="1"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D155" s="1"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D156" s="1"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D157" s="1"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D158" s="1"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D159" s="1"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D160" s="1"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D161" s="1"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D162" s="1"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D163" s="1"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D164" s="1"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D165" s="1"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D166" s="1"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D167" s="1"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D168" s="1"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D169" s="1"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D170" s="1"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D171" s="1"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D172" s="1"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D173" s="1"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D174" s="1"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D175" s="1"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D176" s="1"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D177" s="1"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D178" s="1"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D179" s="1"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D180" s="1"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D181" s="1"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D182" s="1"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D183" s="1"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D184" s="1"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D185" s="1"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D186" s="1"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D187" s="1"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D188" s="1"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D189" s="1"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D190" s="1"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D191" s="1"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D192" s="1"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D193" s="1"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D194" s="1"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D195" s="1"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D196" s="1"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D197" s="1"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D198" s="1"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D199" s="1"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D200" s="1"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D201" s="1"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D202" s="1"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D203" s="1"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D204" s="1"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D205" s="1"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D206" s="1"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D207" s="1"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D208" s="1"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D209" s="1"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D210" s="1"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D211" s="1"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D212" s="1"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D213" s="1"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D214" s="1"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D215" s="1"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D216" s="1"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D217" s="1"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D218" s="1"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D219" s="1"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D220" s="1"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D221" s="1"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D222" s="1"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D223" s="1"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D224" s="1"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D225" s="1"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D226" s="1"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D227" s="1"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D228" s="1"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D229" s="1"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D230" s="1"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D231" s="1"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D232" s="1"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D233" s="1"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D234" s="1"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D235" s="1"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D236" s="1"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D237" s="1"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D238" s="1"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D239" s="1"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D240" s="1"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D241" s="1"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D242" s="1"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D243" s="1"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D244" s="1"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D245" s="1"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D246" s="1"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D247" s="1"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D248" s="1"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D249" s="1"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D250" s="1"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D251" s="1"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D252" s="1"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D253" s="1"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D254" s="1"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D255" s="1"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D256" s="1"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D257" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>